<commit_message>
Update definition of #7
</commit_message>
<xml_diff>
--- a/assets/other/ProjectList.xlsx
+++ b/assets/other/ProjectList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITfiles\JDI-GitHub-website\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0D6C9954-1CF5-4043-A008-E677C79C5DC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{579BEF68-5D0C-4D30-BFA0-68F060F0CAFE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3195" windowWidth="15330" windowHeight="7890" xr2:uid="{EFEE3E06-8E7A-4EB9-AA9F-24DD4063BC3F}"/>
+    <workbookView xWindow="0" yWindow="3645" windowWidth="15330" windowHeight="7890" xr2:uid="{EFEE3E06-8E7A-4EB9-AA9F-24DD4063BC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
     <t>inProgress</t>
   </si>
   <si>
-    <t>on-line version of the popular rock-paper-scissors game. In this version you will be able to play the game or to just "watch" other people play. Or, if a spot is available, you can play the game against someone else.</t>
+    <t>On-line version of the popular rock-paper-scissors game. In this version you will be able to just "watch" other people play or, if a spot is available, you can play the game against someone else.</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="9.140625" style="3"/>
     <col min="3" max="3" width="34.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="57.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="2"/>
@@ -702,7 +702,7 @@
         <v>var project6 = new projectX('6: GifTastic', 'Aynamic web page that populates gifs of your choice using the GIPHY API. This project uses API calls to GIPHY and modifies the DOM using JavaScript and jQuery', 'giphy', 'done');</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>7</v>
       </c>
@@ -720,7 +720,7 @@
       </c>
       <c r="H8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>var project7 = new projectX('7: Rock Paper Scissors', 'on-line version of the popular rock-paper-scissors game. In this version you will be able to play the game or to just "watch" other people play. Or, if a spot is available, you can play the game against someone else.', 'RPS-Multiplayer', 'inProgress');</v>
+        <v>var project7 = new projectX('7: Rock Paper Scissors', 'On-line version of the popular rock-paper-scissors game. In this version you will be able to just "watch" other people play or, if a spot is available, you can play the game against someone else.', 'RPS-Multiplayer', 'inProgress');</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update project #8 LIRI
</commit_message>
<xml_diff>
--- a/assets/other/ProjectList.xlsx
+++ b/assets/other/ProjectList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITfiles\JDI-GitHub-website\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F0472D-D70E-4548-8B32-BFA5491D4D71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60900CB7-D527-4956-9014-A5462457DC50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4545" windowWidth="15330" windowHeight="7890" xr2:uid="{EFEE3E06-8E7A-4EB9-AA9F-24DD4063BC3F}"/>
+    <workbookView xWindow="0" yWindow="4995" windowWidth="15330" windowHeight="7890" xr2:uid="{EFEE3E06-8E7A-4EB9-AA9F-24DD4063BC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>1: Building a Wireframe / That Portfolio Though</t>
   </si>
@@ -152,10 +152,13 @@
     <t>project1</t>
   </si>
   <si>
-    <t>inProgress</t>
-  </si>
-  <si>
     <t>FLIP.IMG - Superhero image matching game. Our web version of the popular memory card game where the objective is to collect the most pairs of cards.</t>
+  </si>
+  <si>
+    <t>This project is a LIRI (Language Interpretation and Recognition Interface); a command line node app that takes in parameters and gives you back data.</t>
+  </si>
+  <si>
+    <t>liri-node-app</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,19 +740,25 @@
         <v>var project7 = new projectX('7: Rock Paper Scissors', 'On-line version of the popular rock-paper-scissors game. In this version you will be able to just "watch" other people play or, if a spot is available, you can play the game against someone else.', 'RPS-Multiplayer', 'done');</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="H9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>var project8 = new projectX('8: LIRI Bot', '', '', 'inProgress');</v>
+        <v>var project8 = new projectX('8: LIRI Bot', 'This project is a LIRI (Language Interpretation and Recognition Interface); a command line node app that takes in parameters and gives you back data.', 'liri-node-app', 'done');</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
@@ -895,7 +904,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>39</v>

</xml_diff>